<commit_message>
added abcdefgh to excel spreadsheet
</commit_message>
<xml_diff>
--- a/testspreadsheet.xlsx
+++ b/testspreadsheet.xlsx
@@ -21,6 +21,43 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,56 +419,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:C10"/>
+  <dimension ref="C3:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>